<commit_message>
list the transactions with column names changed
</commit_message>
<xml_diff>
--- a/Rohan/data/income.xlsx
+++ b/Rohan/data/income.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c1c741db71da0312/Desktop/VS Code Github/python-project/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c1c741db71da0312/Desktop/VS Code Github/python-project/Rohan/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_2B59D2BFD3B058C38C891FD04BFD68B47803FF52" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9DCE435D-CD34-4CFA-A198-E66B90612195}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="11_2B59D2BFD3B058C38C891FD04BFD68B47803FF52" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0B911DE7-714E-4193-8C80-4F2C7EF1C160}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,24 +22,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="15">
   <si>
-    <t>income_id</t>
-  </si>
-  <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>category</t>
-  </si>
-  <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>amount</t>
-  </si>
-  <si>
-    <t>transaction_id</t>
-  </si>
-  <si>
     <t>Salary</t>
   </si>
   <si>
@@ -65,6 +47,24 @@
   </si>
   <si>
     <t>Graphic Design for SAF</t>
+  </si>
+  <si>
+    <t>Income ID</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Transaction ID</t>
   </si>
 </sst>
 </file>
@@ -72,7 +72,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="dd\-mm\-yyyy"/>
+    <numFmt numFmtId="164" formatCode="dd\-mm\-yyyy"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -128,7 +128,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -434,49 +434,49 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="20.6328125" customWidth="1"/>
+    <col min="5" max="5" width="20.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>2500</v>
+      </c>
+      <c r="E2" s="2">
         <v>45658</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2">
-        <v>2500</v>
       </c>
       <c r="F2">
         <v>5</v>
@@ -486,17 +486,17 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>1000</v>
+      </c>
+      <c r="E3" s="2">
         <v>45767</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3">
-        <v>1000</v>
       </c>
       <c r="F3">
         <v>44</v>
@@ -506,17 +506,17 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>102.2</v>
+      </c>
+      <c r="E4" s="2">
         <v>45688</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4">
-        <v>102.2</v>
       </c>
       <c r="F4">
         <v>74</v>
@@ -526,17 +526,17 @@
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>2500</v>
+      </c>
+      <c r="E5" s="2">
         <v>45689</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5">
-        <v>2500</v>
       </c>
       <c r="F5">
         <v>78</v>
@@ -546,17 +546,17 @@
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6">
+        <v>288</v>
+      </c>
+      <c r="E6" s="2">
         <v>45702</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6">
-        <v>288</v>
       </c>
       <c r="F6">
         <v>100</v>
@@ -566,17 +566,17 @@
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>58.7</v>
+      </c>
+      <c r="E7" s="2">
         <v>45716</v>
-      </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7">
-        <v>58.7</v>
       </c>
       <c r="F7">
         <v>134</v>
@@ -586,17 +586,17 @@
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>2500</v>
+      </c>
+      <c r="E8" s="2">
         <v>45717</v>
-      </c>
-      <c r="C8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8">
-        <v>2500</v>
       </c>
       <c r="F8">
         <v>137</v>
@@ -606,17 +606,17 @@
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9">
+        <v>17.010000000000002</v>
+      </c>
+      <c r="E9" s="2">
         <v>45747</v>
-      </c>
-      <c r="C9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9">
-        <v>17.010000000000002</v>
       </c>
       <c r="F9">
         <v>211</v>
@@ -626,17 +626,17 @@
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>2500</v>
+      </c>
+      <c r="E10" s="2">
         <v>45748</v>
-      </c>
-      <c r="C10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10">
-        <v>2500</v>
       </c>
       <c r="F10">
         <v>216</v>
@@ -646,17 +646,17 @@
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="2">
-        <v>45767</v>
+      <c r="B11" t="s">
+        <v>2</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
       </c>
-      <c r="D11" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11">
+      <c r="D11">
         <v>1000</v>
+      </c>
+      <c r="E11" s="2">
+        <v>45767</v>
       </c>
       <c r="F11">
         <v>251</v>
@@ -666,17 +666,17 @@
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12">
+        <v>45.67</v>
+      </c>
+      <c r="E12" s="2">
         <v>45777</v>
-      </c>
-      <c r="C12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12">
-        <v>45.67</v>
       </c>
       <c r="F12">
         <v>278</v>

</xml_diff>